<commit_message>
Se actualiza el diccionario, y se agregan los parametros de conocimiento de personajes y cualidades de candidatos
</commit_message>
<xml_diff>
--- a/data-raw/diccionario_enc_chih_dic_2024.xlsx
+++ b/data-raw/diccionario_enc_chih_dic_2024.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="245">
   <si>
     <t>bloque</t>
   </si>
@@ -176,31 +176,58 @@
     <t>cali_delincuencia</t>
   </si>
   <si>
+    <t>Delincuencia</t>
+  </si>
+  <si>
     <t>1_2_3_4_5_6_7_Ns/Nc</t>
   </si>
   <si>
     <t>cali_educacion</t>
   </si>
   <si>
+    <t>Educación</t>
+  </si>
+  <si>
     <t>cali_salud</t>
   </si>
   <si>
+    <t>Salud</t>
+  </si>
+  <si>
     <t>cali_empleo</t>
   </si>
   <si>
+    <t>Empleo</t>
+  </si>
+  <si>
     <t>cali_pensiones</t>
   </si>
   <si>
+    <t>Pensiones</t>
+  </si>
+  <si>
     <t>cali_ambiente</t>
   </si>
   <si>
+    <t>Medio ambiente</t>
+  </si>
+  <si>
     <t>cali_inmigracion</t>
   </si>
   <si>
+    <t>Inmigración</t>
+  </si>
+  <si>
     <t>cali_derechosmujer</t>
   </si>
   <si>
+    <t>Derechos para la mujer</t>
+  </si>
+  <si>
     <t>cali_economia</t>
+  </si>
+  <si>
+    <t>Economía</t>
   </si>
   <si>
     <t>¿Usted cree que en el momento actual Chile está: progresando, estancado o en
@@ -1404,9 +1431,11 @@
       <c r="D22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="F22" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23">
@@ -1420,11 +1449,13 @@
         <v>15</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="24">
@@ -1438,11 +1469,13 @@
         <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="F24" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25">
@@ -1456,11 +1489,13 @@
         <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="F25" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26">
@@ -1474,11 +1509,13 @@
         <v>15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="F26" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27">
@@ -1492,11 +1529,13 @@
         <v>15</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E27" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F27" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28">
@@ -1510,11 +1549,13 @@
         <v>15</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="F28" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29">
@@ -1528,11 +1569,13 @@
         <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F29" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30">
@@ -1546,11 +1589,13 @@
         <v>15</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="F30" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31">
@@ -1558,17 +1603,17 @@
         <v>24</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32">
@@ -1576,17 +1621,17 @@
         <v>24</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33">
@@ -1594,17 +1639,17 @@
         <v>24</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34">
@@ -1612,17 +1657,17 @@
         <v>24</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35">
@@ -1630,17 +1675,17 @@
         <v>24</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36">
@@ -1648,17 +1693,17 @@
         <v>24</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37">
@@ -1666,17 +1711,17 @@
         <v>24</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38">
@@ -1684,17 +1729,17 @@
         <v>24</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39">
@@ -1702,17 +1747,17 @@
         <v>24</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40">
@@ -1720,34 +1765,34 @@
         <v>24</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>21</v>
@@ -1755,19 +1800,19 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>21</v>
@@ -1775,19 +1820,19 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>21</v>
@@ -1795,19 +1840,19 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>21</v>
@@ -1815,19 +1860,19 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>21</v>
@@ -1835,19 +1880,19 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>21</v>
@@ -1855,19 +1900,19 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>21</v>
@@ -1875,19 +1920,19 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>21</v>
@@ -1895,19 +1940,19 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>21</v>
@@ -1915,664 +1960,664 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="F54" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2" t="s">
@@ -2581,16 +2626,16 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2" t="s">
@@ -2599,34 +2644,34 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
@@ -2635,446 +2680,446 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="2" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109" s="2" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110" s="2" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111" s="2" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112" s="2" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113" s="2" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114" s="2" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115" s="2" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116" s="2" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="E117" s="2"/>
       <c r="F117" s="2" t="s">
@@ -3083,16 +3128,16 @@
     </row>
     <row r="118">
       <c r="A118" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118" s="2" t="s">
@@ -3101,38 +3146,38 @@
     </row>
     <row r="119">
       <c r="A119" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119" s="2" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120" s="2" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se adaptan los scripts para las nubes, se crea el script para comparar sexo y edad encuesta y real, se crean las bases para comaprar la data. se hacen cambios correspondientes
</commit_message>
<xml_diff>
--- a/data-raw/diccionario_enc_chih_dic_2024.xlsx
+++ b/data-raw/diccionario_enc_chih_dic_2024.xlsx
@@ -310,7 +310,7 @@
     <t>conoce_per_bachelet</t>
   </si>
   <si>
-    <t>Michelle Bachellete</t>
+    <t>Michelle Bachelete</t>
   </si>
   <si>
     <t>conoce_per_winter</t>
@@ -1050,7 +1050,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="22.13"/>
     <col customWidth="1" min="2" max="2" width="76.38"/>
-    <col customWidth="1" min="4" max="4" width="26.38"/>
+    <col customWidth="1" min="4" max="4" width="6.5"/>
     <col customWidth="1" min="5" max="5" width="15.38"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
se agregan pca y cruce de voto_pr y voto2_pr
</commit_message>
<xml_diff>
--- a/data-raw/diccionario_enc_chih_dic_2024.xlsx
+++ b/data-raw/diccionario_enc_chih_dic_2024.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="247">
   <si>
     <t>bloque</t>
   </si>
@@ -604,10 +604,16 @@
 decir tres cualidades, por favor.</t>
   </si>
   <si>
-    <t>cualidades_valora_candidato</t>
+    <t>cualidades_valora_candidato_O1</t>
   </si>
   <si>
     <t>Conciliador, genera diálogos y acuerdos_Preparación profesional, culto_Experiencia política_Consecuente entre lo que dice y lo que hace_Intachable, sin historial de corrupción_Empresario, conocimientos de economía_Cercano a la gente, involucrado en la calle_Buen orador_Con carácter, con autoridad_Perseverante o persistente_Sólido o seguro de convicciones_Que vista bien, buena facha_Otro:_Ns/Nc (No leer)</t>
+  </si>
+  <si>
+    <t>cualidades_valora_candidato_O2</t>
+  </si>
+  <si>
+    <t>cualidades_valora_candidato_O3</t>
   </si>
   <si>
     <t>otro_cualidades_valora_candidato</t>
@@ -2868,10 +2874,14 @@
         <v>191</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>194</v>
+      </c>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="104">
@@ -2879,17 +2889,17 @@
         <v>190</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D104" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="105">
@@ -2897,287 +2907,319 @@
         <v>190</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>203</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="E106" s="2"/>
       <c r="F106" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>206</v>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E110" s="2"/>
+      <c r="E110" s="2" t="s">
+        <v>211</v>
+      </c>
       <c r="F110" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E117" s="2"/>
       <c r="F117" s="2" t="s">
-        <v>21</v>
+        <v>233</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118" s="2" t="s">
-        <v>21</v>
+        <v>236</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119" s="2" t="s">
-        <v>241</v>
+        <v>21</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>244</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>